<commit_message>
feat: add lv_games and update hardware
</commit_message>
<xml_diff>
--- a/hardware/BOM_PCB_基于ESP32S3的智能终端.xlsx
+++ b/hardware/BOM_PCB_基于ESP32S3的智能终端.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A504C2F6-941D-4856-9B68-193EBE1AF850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D1C94D-45AB-4568-8F42-954CFC41D2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>C3,C5,C6,C11,C12,C19</t>
   </si>
@@ -65,9 +62,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>U9</t>
-  </si>
-  <si>
     <t>USB1</t>
   </si>
   <si>
@@ -83,18 +77,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://item.taobao.com/item.htm?id=556985020016&amp;mi_id=0000eN4V-uiZA5WsXTJMXxgHSsvGZr2dQiXve435ROzxwsA&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOOT,RST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2*4*3.5_侧按贴片2脚_散装(20只)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C1,C2，C4,C7,C8,C9,C10,C15,C16,C17,C18,C20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -180,10 +166,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://item.taobao.com/item.htm?id=552732254981&amp;mi_id=000045agQIeAYvQjfpMgfvG0Psgxbrr1qn44v2KAYf0pCvU&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10P 翻盖下接</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -313,14 +295,6 @@
   </si>
   <si>
     <t>NS4168功放芯片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://item.taobao.com/item.htm?id=930040367194&amp;mi_id=0000XKRhs9PqKjZ7VOgMX2rvPF8gcrXToUiClPzYnZ79k18&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INMP441麦克风模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -380,10 +354,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R1,R8,R11,R17,R20,R21,R22,R23,R24,R25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0603贴片电阻 1K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -433,6 +403,33 @@
   </si>
   <si>
     <t>红色 503450(1000mah) 找客服备注接口2.0反向黑红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1,R8,R11,R17,R20,R21,R22,R23,R24,R26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?id=552629356951&amp;pisk=fFBZGEZVFReahOasNFJq4Hv9IOv9_LUWItTXmijDfFYM5t_VmntvjnDDiDvHmeMbXdNv3Z8FkFO6IFM23i7AlIXXltoOLakjCPFOmxJXnza7F8sOfKp0P0outx394nK0hnYMth8jCua7F8sEtYTUYz1_7Xokan9DjFvDtk-2jhvDsIA3YnxjSEYGoMcIT1humoAu7gYh1VpXN4r1sekmU0KwsLwJ-xDcLhS6rGVxnxXebCWFJB0i8C1c2QB1A-kpCg5HK3sTQvJlj376Ra2oLpjCxZOR9rHW9wW2wOAimkYhQwW9INNmUaJNuQXMTmDfjMY9LHXucbLCLF_cQBqSUI9hFQvGOWU6Gd-PoOQZ0xbl403vx-VfH1umgCxpYUZUYGVCdyJQp77qMjdOwH87XuGxMCxpYUZUYjhv6dxePlE5.&amp;spm=a1z10.3-c-s.w4002-24706531953.10.6ac36a4bzX7DWm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?abbucket=7&amp;id=721849788406&amp;mi_id=0000i-9kflJwjnoKfd-ULIsY0OrhOOrEK7mUPc35AmdH8LM&amp;ns=1&amp;priceTId=2150485917639114151111852e1738&amp;skuId=5196908507751&amp;spm=a21n57.1.hoverItem.2&amp;utparam=%7B%22aplus_abtest%22%3A%22c1e568057aafdfecd926915830b4f7b5%22%7D&amp;xxc=taobaoSearch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSM261S4030H0R麦克风芯片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轻触开关4.5*4.5*3.8/4.3/4.8/5/6/8MM边三脚按键 侧插侧按边三角-淘宝网</t>
+  </si>
+  <si>
+    <t>4.5*4.5*8三角侧按键</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -847,12 +844,12 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
     <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="3" max="3" width="46.88671875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
@@ -860,447 +857,447 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{367EC601-2F23-4EF9-AD51-2F7CDC944FAE}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://item.taobao.com/item.htm?id=560886805480&amp;mi_id=0000u9Wqn90ydQ-JS4at8R0B65ukrE8VNK7rOw-bkwAOYcU&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{9E928C85-C511-426F-B527-4C8045EAC04B}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://item.taobao.com/item.htm?id=620467815833&amp;mi_id=0000w1hW6eprvVw_thtIdD0xoczgRSlqp9nLyU0WaZUvF3U&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{73471DEA-87B6-4908-BC9D-A5E5D53CEAA3}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://item.taobao.com/item.htm?id=537706477476&amp;mi_id=0000-qrJZDSABENB-W7E1uICfBYbdyr5O13nW5AhDZJ6Uik&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{0982F950-C2F8-429D-86C3-22C1B68463A1}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{567B7AB3-CC0E-4FB0-A319-4891D82BE56D}"/>
-    <hyperlink ref="B5" r:id="rId6" display="https://item.taobao.com/item.htm?id=536850914586&amp;pisk=g8I-WcT_dSVlISGre640-ezkdx2DyrXzM_WsxBAoRsCAd_OktUOWcE9yKX9WN99Bvs13UQXQa6IpG97uUeVrpZCPCUfdL8JBO61pta40jTWyYHNM9lqGU7lWL31pPUTfhtJEPLaDPLKx2HVgslqLPxtLw5Xo2UtThdp6ALOWAKwvddpBAUOIl-pBKbOBN66bHIJZFYOBFEZXEIgSVpiIct9kpDgSApwAhIJMAB1BP-BXgptBOvDtpBD99DQr0WO-kckKxDjveUdKxInL0JvWys6JMWPODc8J1TOxA7QkVpdpgGN0kt7fP_vV9lFvYs7COpCjGWYPdZCve_VtTBjPEMdlezNPHnORNUQYC4JAngBdREe7VtKJwFjANv0y2w1PvU7-LRWXVs7w_Ua4gKIljedwkjN5ntdWWwCugDOlWt1vSicmjH5VR69dGbIywGj9ohlM6p07H-3E8U94ZUlPeltkd0Jvs-0i828DKKdgH-3E8U92HC2022ueopf..&amp;spm=a1z10.3-c-s.w4002-24706531953.27.2ef36a4bjgPZK0&amp;skuId=5895612234672" xr:uid="{166E8BA5-8BEE-4CC3-A3D8-48BAF031F71A}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://item.taobao.com/item.htm?abbucket=16&amp;id=992597661298&amp;mi_id=0000w_wSwn1ek9k-ZvmM2NNucf8C5QSzViDTZemY-ZW7-HM&amp;ns=1&amp;priceTId=215049d217631278934968720e1127&amp;spm=a21n57.1.hoverItem.5&amp;utparam=%7B%22aplus_abtest%22%3A%22b722ed98aba1e56ea2418ccc277051e6%22%7D&amp;xxc=taobaoSearch&amp;sku_properties=5919063%3A6536025" xr:uid="{5A6BB97B-0D10-4CA1-96B6-27551BF38FE3}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{17752616-DD40-45F8-89D0-DB8418AFE8FC}"/>
-    <hyperlink ref="B11" r:id="rId9" xr:uid="{9600EBBF-AEB4-4709-B471-7519E964A609}"/>
-    <hyperlink ref="B13" r:id="rId10" xr:uid="{4E442B27-AD1E-4E8E-BC9A-5CFD50BF8B96}"/>
-    <hyperlink ref="B15" r:id="rId11" xr:uid="{DA08EDF0-9928-451F-91AE-AA3B3561B5FA}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{4D762C97-F9F3-41D5-AFA5-272A7A7C9FD5}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{0B49417B-4DBF-4994-95E0-EA43AA5E7B3E}"/>
-    <hyperlink ref="B25" r:id="rId14" xr:uid="{F2B17918-F1CD-4A3F-8ED9-20ACA8F823E2}"/>
-    <hyperlink ref="B26" r:id="rId15" xr:uid="{A649C5BF-C17C-4198-B2B7-96EA8D21B718}"/>
-    <hyperlink ref="B28" r:id="rId16" xr:uid="{19D1A1AE-F435-477D-8E69-4598E680D90B}"/>
-    <hyperlink ref="B29" r:id="rId17" xr:uid="{2457B954-BCC2-4063-B59A-B4686787F27D}"/>
-    <hyperlink ref="B30" r:id="rId18" xr:uid="{78A56D3C-9934-4BED-BB68-683649A21603}"/>
-    <hyperlink ref="B31" r:id="rId19" xr:uid="{4399402F-AC4A-44B8-8F24-C0E63462FFE4}"/>
-    <hyperlink ref="B32" r:id="rId20" xr:uid="{ECA04BE2-1916-405F-8354-A6345AE29F9C}"/>
-    <hyperlink ref="B33" r:id="rId21" xr:uid="{A458F1A6-1F58-40DF-B405-89202C010D84}"/>
-    <hyperlink ref="B34" r:id="rId22" xr:uid="{03CE4BFB-59E7-466D-8602-7F91E301DE7B}"/>
-    <hyperlink ref="B35" r:id="rId23" xr:uid="{CDDC7513-93F0-411F-9514-4D13DBEC2629}"/>
-    <hyperlink ref="B18" r:id="rId24" xr:uid="{6C3C89F2-67B6-4795-A00D-61609CC6DDB0}"/>
-    <hyperlink ref="B22" r:id="rId25" xr:uid="{0742B95A-1BF5-4AFE-A3F1-0E97F27FA66D}"/>
-    <hyperlink ref="B23" r:id="rId26" xr:uid="{23E99429-6AEB-4841-84B4-617F2F475168}"/>
-    <hyperlink ref="B24" r:id="rId27" xr:uid="{BC492E97-CE0B-461C-A191-E175FC6FE53F}"/>
-    <hyperlink ref="B19" r:id="rId28" xr:uid="{DA3A4F05-0016-4C21-BA35-EAEEF7436120}"/>
-    <hyperlink ref="B17" r:id="rId29" xr:uid="{7F2C983B-3521-459E-85A3-E268D5132C31}"/>
-    <hyperlink ref="B20" r:id="rId30" xr:uid="{7C94672B-57F0-4A16-9E53-FCDC95556EDA}"/>
-    <hyperlink ref="B21" r:id="rId31" xr:uid="{45E3AB37-9F55-401F-A5EF-87CFF72AB71F}"/>
-    <hyperlink ref="B36" r:id="rId32" xr:uid="{034637B1-1868-4BBB-8572-C21BAEDE1138}"/>
-    <hyperlink ref="B37" r:id="rId33" xr:uid="{3C711CC2-01F8-4A6D-A496-CD1B1FA1B486}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://item.taobao.com/item.htm?id=560886805480&amp;mi_id=0000u9Wqn90ydQ-JS4at8R0B65ukrE8VNK7rOw-bkwAOYcU&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{9E928C85-C511-426F-B527-4C8045EAC04B}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://item.taobao.com/item.htm?id=620467815833&amp;mi_id=0000w1hW6eprvVw_thtIdD0xoczgRSlqp9nLyU0WaZUvF3U&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{73471DEA-87B6-4908-BC9D-A5E5D53CEAA3}"/>
+    <hyperlink ref="B6" r:id="rId3" display="https://item.taobao.com/item.htm?id=537706477476&amp;mi_id=0000-qrJZDSABENB-W7E1uICfBYbdyr5O13nW5AhDZJ6Uik&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.3d8f2e8dMW9QnL" xr:uid="{0982F950-C2F8-429D-86C3-22C1B68463A1}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{567B7AB3-CC0E-4FB0-A319-4891D82BE56D}"/>
+    <hyperlink ref="B5" r:id="rId5" display="https://item.taobao.com/item.htm?id=536850914586&amp;pisk=g8I-WcT_dSVlISGre640-ezkdx2DyrXzM_WsxBAoRsCAd_OktUOWcE9yKX9WN99Bvs13UQXQa6IpG97uUeVrpZCPCUfdL8JBO61pta40jTWyYHNM9lqGU7lWL31pPUTfhtJEPLaDPLKx2HVgslqLPxtLw5Xo2UtThdp6ALOWAKwvddpBAUOIl-pBKbOBN66bHIJZFYOBFEZXEIgSVpiIct9kpDgSApwAhIJMAB1BP-BXgptBOvDtpBD99DQr0WO-kckKxDjveUdKxInL0JvWys6JMWPODc8J1TOxA7QkVpdpgGN0kt7fP_vV9lFvYs7COpCjGWYPdZCve_VtTBjPEMdlezNPHnORNUQYC4JAngBdREe7VtKJwFjANv0y2w1PvU7-LRWXVs7w_Ua4gKIljedwkjN5ntdWWwCugDOlWt1vSicmjH5VR69dGbIywGj9ohlM6p07H-3E8U94ZUlPeltkd0Jvs-0i828DKKdgH-3E8U92HC2022ueopf..&amp;spm=a1z10.3-c-s.w4002-24706531953.27.2ef36a4bjgPZK0&amp;skuId=5895612234672" xr:uid="{166E8BA5-8BEE-4CC3-A3D8-48BAF031F71A}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://item.taobao.com/item.htm?abbucket=16&amp;id=992597661298&amp;mi_id=0000w_wSwn1ek9k-ZvmM2NNucf8C5QSzViDTZemY-ZW7-HM&amp;ns=1&amp;priceTId=215049d217631278934968720e1127&amp;spm=a21n57.1.hoverItem.5&amp;utparam=%7B%22aplus_abtest%22%3A%22b722ed98aba1e56ea2418ccc277051e6%22%7D&amp;xxc=taobaoSearch&amp;sku_properties=5919063%3A6536025" xr:uid="{5A6BB97B-0D10-4CA1-96B6-27551BF38FE3}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://item.taobao.com/item.htm?id=552629356951&amp;pisk=fFBZGEZVFReahOasNFJq4Hv9IOv9_LUWItTXmijDfFYM5t_VmntvjnDDiDvHmeMbXdNv3Z8FkFO6IFM23i7AlIXXltoOLakjCPFOmxJXnza7F8sOfKp0P0outx394nK0hnYMth8jCua7F8sEtYTUYz1_7Xokan9DjFvDtk-2jhvDsIA3YnxjSEYGoMcIT1humoAu7gYh1VpXN4r1sekmU0KwsLwJ-xDcLhS6rGVxnxXebCWFJB0i8C1c2QB1A-kpCg5HK3sTQvJlj376Ra2oLpjCxZOR9rHW9wW2wOAimkYhQwW9INNmUaJNuQXMTmDfjMY9LHXucbLCLF_cQBqSUI9hFQvGOWU6Gd-PoOQZ0xbl403vx-VfH1umgCxpYUZUYGVCdyJQp77qMjdOwH87XuGxMCxpYUZUYjhv6dxePlE5.&amp;spm=a1z10.3-c-s.w4002-24706531953.10.6ac36a4bzX7DWm" xr:uid="{17752616-DD40-45F8-89D0-DB8418AFE8FC}"/>
+    <hyperlink ref="B13" r:id="rId8" xr:uid="{4E442B27-AD1E-4E8E-BC9A-5CFD50BF8B96}"/>
+    <hyperlink ref="B15" r:id="rId9" xr:uid="{DA08EDF0-9928-451F-91AE-AA3B3561B5FA}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{4D762C97-F9F3-41D5-AFA5-272A7A7C9FD5}"/>
+    <hyperlink ref="B16" r:id="rId11" xr:uid="{0B49417B-4DBF-4994-95E0-EA43AA5E7B3E}"/>
+    <hyperlink ref="B25" r:id="rId12" xr:uid="{F2B17918-F1CD-4A3F-8ED9-20ACA8F823E2}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{A649C5BF-C17C-4198-B2B7-96EA8D21B718}"/>
+    <hyperlink ref="B28" r:id="rId14" xr:uid="{19D1A1AE-F435-477D-8E69-4598E680D90B}"/>
+    <hyperlink ref="B29" r:id="rId15" xr:uid="{2457B954-BCC2-4063-B59A-B4686787F27D}"/>
+    <hyperlink ref="B30" r:id="rId16" xr:uid="{78A56D3C-9934-4BED-BB68-683649A21603}"/>
+    <hyperlink ref="B31" r:id="rId17" xr:uid="{4399402F-AC4A-44B8-8F24-C0E63462FFE4}"/>
+    <hyperlink ref="B32" r:id="rId18" xr:uid="{ECA04BE2-1916-405F-8354-A6345AE29F9C}"/>
+    <hyperlink ref="B33" r:id="rId19" xr:uid="{A458F1A6-1F58-40DF-B405-89202C010D84}"/>
+    <hyperlink ref="B35" r:id="rId20" xr:uid="{CDDC7513-93F0-411F-9514-4D13DBEC2629}"/>
+    <hyperlink ref="B18" r:id="rId21" xr:uid="{6C3C89F2-67B6-4795-A00D-61609CC6DDB0}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{0742B95A-1BF5-4AFE-A3F1-0E97F27FA66D}"/>
+    <hyperlink ref="B23" r:id="rId23" xr:uid="{23E99429-6AEB-4841-84B4-617F2F475168}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{BC492E97-CE0B-461C-A191-E175FC6FE53F}"/>
+    <hyperlink ref="B19" r:id="rId25" xr:uid="{DA3A4F05-0016-4C21-BA35-EAEEF7436120}"/>
+    <hyperlink ref="B17" r:id="rId26" xr:uid="{7F2C983B-3521-459E-85A3-E268D5132C31}"/>
+    <hyperlink ref="B20" r:id="rId27" xr:uid="{7C94672B-57F0-4A16-9E53-FCDC95556EDA}"/>
+    <hyperlink ref="B21" r:id="rId28" xr:uid="{45E3AB37-9F55-401F-A5EF-87CFF72AB71F}"/>
+    <hyperlink ref="B36" r:id="rId29" xr:uid="{034637B1-1868-4BBB-8572-C21BAEDE1138}"/>
+    <hyperlink ref="B37" r:id="rId30" xr:uid="{3C711CC2-01F8-4A6D-A496-CD1B1FA1B486}"/>
+    <hyperlink ref="B11" r:id="rId31" display="https://item.taobao.com/item.htm?id=552629356951&amp;pisk=fFBZGEZVFReahOasNFJq4Hv9IOv9_LUWItTXmijDfFYM5t_VmntvjnDDiDvHmeMbXdNv3Z8FkFO6IFM23i7AlIXXltoOLakjCPFOmxJXnza7F8sOfKp0P0outx394nK0hnYMth8jCua7F8sEtYTUYz1_7Xokan9DjFvDtk-2jhvDsIA3YnxjSEYGoMcIT1humoAu7gYh1VpXN4r1sekmU0KwsLwJ-xDcLhS6rGVxnxXebCWFJB0i8C1c2QB1A-kpCg5HK3sTQvJlj376Ra2oLpjCxZOR9rHW9wW2wOAimkYhQwW9INNmUaJNuQXMTmDfjMY9LHXucbLCLF_cQBqSUI9hFQvGOWU6Gd-PoOQZ0xbl403vx-VfH1umgCxpYUZUYGVCdyJQp77qMjdOwH87XuGxMCxpYUZUYjhv6dxePlE5.&amp;spm=a1z10.3-c-s.w4002-24706531953.10.6ac36a4bzX7DWm" xr:uid="{8ED61254-B800-472E-AF91-4ABDC0D92CD6}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://item.taobao.com/item.htm?abbucket=7&amp;id=721849788406&amp;mi_id=0000i-9kflJwjnoKfd-ULIsY0OrhOOrEK7mUPc35AmdH8LM&amp;ns=1&amp;priceTId=2150485917639114151111852e1738&amp;skuId=5196908507751&amp;spm=a21n57.1.hoverItem.2&amp;utparam=%7B%22aplus_abtest%22%3A%22c1e568057aafdfecd926915830b4f7b5%22%7D&amp;xxc=taobaoSearch" xr:uid="{03CE4BFB-59E7-466D-8602-7F91E301DE7B}"/>
+    <hyperlink ref="B2" r:id="rId33" display="https://item.taobao.com/item.htm?abbucket=16&amp;id=566056459966&amp;mi_id=0000BLdnAreZ4nQ-2a76uVNsgSwJ7Bmx1Ka7WZInIiM5HEc&amp;ns=1&amp;priceTId=2150421b17639115789987017e1c0b&amp;skuId=3589998161638&amp;spm=a21n57.1.hoverItem.5&amp;utparam=%7B%22aplus_abtest%22%3A%22f31c0b56be10e20579f9a5cd1edda130%22%7D&amp;xxc=taobaoSearch" xr:uid="{4FD24B14-B9CB-48B7-8008-659E998AB7EC}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>